<commit_message>
Made the test data agnostic to the input excel file. The test for the methods still relies on the existance of the CompositionGraphMaster.json file residing in the data directory. changed the name of the rename_excel_columns() method to rename_columns() since the function name was disingenuous as it operated on a dataframe and not the excel file.
</commit_message>
<xml_diff>
--- a/data/Composition Example.xlsx
+++ b/data/Composition Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bc151\Documents\Toolsmithing\Ingrid Nerdman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Component</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Mount</t>
+  </si>
+  <si>
+    <t>engine</t>
   </si>
 </sst>
 </file>
@@ -410,17 +413,17 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,19 +434,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="str">
-        <f>LOWER(C2)</f>
-        <v>engine</v>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -455,7 +457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -467,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -478,7 +480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -489,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -500,7 +502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -511,7 +513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -523,7 +525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -535,7 +537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -547,7 +549,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -558,7 +560,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -569,7 +571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -580,7 +582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -591,7 +593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -603,7 +605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -615,43 +617,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>